<commit_message>
Added HabilisX.Tex and continue to edit
</commit_message>
<xml_diff>
--- a/HabilisX/890/HabilisData.xlsx
+++ b/HabilisX/890/HabilisData.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PrairieRose\Documents\GitHub\HabilisX\HabilisX\890\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="150" windowWidth="20115" windowHeight="9525" activeTab="3"/>
+    <workbookView xWindow="480" yWindow="156" windowWidth="12480" windowHeight="9528" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet7" sheetId="7" r:id="rId1"/>
@@ -12,7 +17,7 @@
     <sheet name="Sheet13" sheetId="13" r:id="rId3"/>
     <sheet name="Sheet1" sheetId="1" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -267,6 +272,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -439,20 +447,21 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="80975744"/>
-        <c:axId val="80977280"/>
+        <c:axId val="288729032"/>
+        <c:axId val="288725112"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="80975744"/>
+        <c:axId val="288729032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="80977280"/>
+        <c:crossAx val="288725112"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -460,7 +469,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="80977280"/>
+        <c:axId val="288725112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -471,7 +480,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="80975744"/>
+        <c:crossAx val="288729032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -647,20 +656,21 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="82850560"/>
-        <c:axId val="82852096"/>
+        <c:axId val="288724720"/>
+        <c:axId val="288723544"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="82850560"/>
+        <c:axId val="288724720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="82852096"/>
+        <c:crossAx val="288723544"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -668,7 +678,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="82852096"/>
+        <c:axId val="288723544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -679,7 +689,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="82850560"/>
+        <c:crossAx val="288724720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -767,7 +777,7 @@
                 <c:formatCode>h:mm</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>0.55980902777777786</c:v>
+                  <c:v>0.5097222222222223</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -818,7 +828,7 @@
                 <c:formatCode>h:mm</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>0.64913194444444444</c:v>
+                  <c:v>0.69921875</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -833,20 +843,21 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="82873728"/>
-        <c:axId val="82879616"/>
+        <c:axId val="288727072"/>
+        <c:axId val="288723936"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="82873728"/>
+        <c:axId val="288727072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="82879616"/>
+        <c:crossAx val="288723936"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -854,7 +865,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="82879616"/>
+        <c:axId val="288723936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -866,7 +877,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="82873728"/>
+        <c:crossAx val="288727072"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1026,7 +1037,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1061,7 +1072,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1276,13 +1287,13 @@
       <selection activeCell="P22" sqref="P22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.5703125" customWidth="1"/>
-    <col min="9" max="9" width="18.85546875" customWidth="1"/>
+    <col min="1" max="1" width="22.5546875" customWidth="1"/>
+    <col min="9" max="9" width="18.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>23</v>
       </c>
@@ -1290,7 +1301,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>24</v>
       </c>
@@ -1298,7 +1309,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>25</v>
       </c>
@@ -1330,7 +1341,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>30</v>
       </c>
@@ -1362,7 +1373,7 @@
         <v>13.839285714285714</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
         <v>31</v>
       </c>
@@ -1394,7 +1405,7 @@
         <v>12.267857142857142</v>
       </c>
     </row>
-    <row r="9" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>32</v>
       </c>
@@ -1402,7 +1413,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>33</v>
       </c>
@@ -1446,7 +1457,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>40</v>
       </c>
@@ -1490,7 +1501,7 @@
         <v>4.6001099366694227</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>41</v>
       </c>
@@ -1522,7 +1533,7 @@
       <c r="N12" s="3"/>
       <c r="O12" s="3"/>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
@@ -1538,7 +1549,7 @@
       <c r="N13" s="3"/>
       <c r="O13" s="3"/>
     </row>
-    <row r="14" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="4" t="s">
         <v>42</v>
       </c>
@@ -1566,7 +1577,7 @@
       <c r="N14" s="4"/>
       <c r="O14" s="4"/>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>23</v>
       </c>
@@ -1574,7 +1585,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="19" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>24</v>
       </c>
@@ -1582,7 +1593,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
         <v>25</v>
       </c>
@@ -1614,7 +1625,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
         <v>30</v>
       </c>
@@ -1646,7 +1657,7 @@
         <v>4.125</v>
       </c>
     </row>
-    <row r="22" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="4" t="s">
         <v>31</v>
       </c>
@@ -1678,7 +1689,7 @@
         <v>5.5535714285714288</v>
       </c>
     </row>
-    <row r="25" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>32</v>
       </c>
@@ -1686,7 +1697,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A26" s="5" t="s">
         <v>33</v>
       </c>
@@ -1730,7 +1741,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
         <v>40</v>
       </c>
@@ -1774,7 +1785,7 @@
         <v>4.6001099366694227</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
         <v>41</v>
       </c>
@@ -1806,7 +1817,7 @@
       <c r="N28" s="3"/>
       <c r="O28" s="3"/>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A29" s="3"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
@@ -1822,7 +1833,7 @@
       <c r="N29" s="3"/>
       <c r="O29" s="3"/>
     </row>
-    <row r="30" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="4" t="s">
         <v>42</v>
       </c>
@@ -1863,19 +1874,19 @@
       <selection sqref="A1:C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.140625" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" customWidth="1"/>
+    <col min="1" max="1" width="19.109375" customWidth="1"/>
+    <col min="3" max="3" width="13.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="5"/>
       <c r="B3" s="5" t="s">
         <v>44</v>
@@ -1884,7 +1895,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>46</v>
       </c>
@@ -1895,7 +1906,7 @@
         <v>13.75</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>29</v>
       </c>
@@ -1906,7 +1917,7 @@
         <v>5.3571428571428568</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>47</v>
       </c>
@@ -1917,7 +1928,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>48</v>
       </c>
@@ -1926,7 +1937,7 @@
       </c>
       <c r="C7" s="3"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>35</v>
       </c>
@@ -1935,7 +1946,7 @@
       </c>
       <c r="C8" s="3"/>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>49</v>
       </c>
@@ -1944,7 +1955,7 @@
       </c>
       <c r="C9" s="3"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>50</v>
       </c>
@@ -1953,7 +1964,7 @@
       </c>
       <c r="C10" s="3"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>51</v>
       </c>
@@ -1962,7 +1973,7 @@
       </c>
       <c r="C11" s="3"/>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>52</v>
       </c>
@@ -1971,7 +1982,7 @@
       </c>
       <c r="C12" s="3"/>
     </row>
-    <row r="13" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="4" t="s">
         <v>53</v>
       </c>
@@ -1993,15 +2004,15 @@
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="5"/>
       <c r="B3" s="5" t="s">
         <v>44</v>
@@ -2010,7 +2021,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>46</v>
       </c>
@@ -2021,7 +2032,7 @@
         <v>13.75</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>29</v>
       </c>
@@ -2032,7 +2043,7 @@
         <v>5.3571428571428568</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>47</v>
       </c>
@@ -2043,7 +2054,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>55</v>
       </c>
@@ -2052,7 +2063,7 @@
       </c>
       <c r="C7" s="3"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>48</v>
       </c>
@@ -2061,7 +2072,7 @@
       </c>
       <c r="C8" s="3"/>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>35</v>
       </c>
@@ -2070,7 +2081,7 @@
       </c>
       <c r="C9" s="3"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>49</v>
       </c>
@@ -2079,7 +2090,7 @@
       </c>
       <c r="C10" s="3"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>50</v>
       </c>
@@ -2088,7 +2099,7 @@
       </c>
       <c r="C11" s="3"/>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>51</v>
       </c>
@@ -2097,7 +2108,7 @@
       </c>
       <c r="C12" s="3"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>52</v>
       </c>
@@ -2106,7 +2117,7 @@
       </c>
       <c r="C13" s="3"/>
     </row>
-    <row r="14" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="4" t="s">
         <v>53</v>
       </c>
@@ -2125,12 +2136,12 @@
   <dimension ref="A1:U30"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C4" workbookViewId="0">
-      <selection activeCell="N2" sqref="N2:O9"/>
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>1</v>
       </c>
@@ -2180,7 +2191,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -2239,7 +2250,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -2298,7 +2309,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -2357,7 +2368,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -2386,10 +2397,10 @@
         <v>10</v>
       </c>
       <c r="K5" s="1">
+        <v>0.55555555555555558</v>
+      </c>
+      <c r="L5" s="1">
         <v>0.95624999999999993</v>
-      </c>
-      <c r="L5" s="1">
-        <v>0.55555555555555558</v>
       </c>
       <c r="N5">
         <v>15</v>
@@ -2416,7 +2427,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -2475,7 +2486,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -2534,7 +2545,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -2593,7 +2604,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -2652,7 +2663,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>16</v>
       </c>
@@ -2672,7 +2683,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>21</v>
       </c>
@@ -2697,14 +2708,14 @@
       </c>
       <c r="K11" s="1">
         <f>AVERAGE(K2:K9)</f>
-        <v>0.55980902777777786</v>
+        <v>0.5097222222222223</v>
       </c>
       <c r="L11" s="1">
         <f>AVERAGE(L2:L9)</f>
-        <v>0.64913194444444444</v>
-      </c>
-    </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+        <v>0.69921875</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>20</v>
       </c>
@@ -2725,7 +2736,7 @@
         <v>5.875</v>
       </c>
     </row>
-    <row r="30" ht="10.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="30" ht="10.5" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Changed legend on figures
</commit_message>
<xml_diff>
--- a/HabilisX/890/HabilisData.xlsx
+++ b/HabilisX/890/HabilisData.xlsx
@@ -87,9 +87,6 @@
     <t>Mendeley</t>
   </si>
   <si>
-    <t>Habilis</t>
-  </si>
-  <si>
     <t>Average Time</t>
   </si>
   <si>
@@ -190,6 +187,9 @@
   </si>
   <si>
     <t>Pearson Correlation</t>
+  </si>
+  <si>
+    <t>Gismo</t>
   </si>
 </sst>
 </file>
@@ -378,7 +378,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Habilis</c:v>
+                  <c:v>Gismo</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -447,11 +447,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="288729032"/>
-        <c:axId val="288725112"/>
+        <c:axId val="301015168"/>
+        <c:axId val="301015560"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="288729032"/>
+        <c:axId val="301015168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -461,7 +461,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="288725112"/>
+        <c:crossAx val="301015560"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -469,7 +469,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="288725112"/>
+        <c:axId val="301015560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -480,7 +480,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="288729032"/>
+        <c:crossAx val="301015168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -532,7 +532,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Habilis</c:v>
+                  <c:v>Gismo</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -656,11 +656,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="288724720"/>
-        <c:axId val="288723544"/>
+        <c:axId val="301016344"/>
+        <c:axId val="301017520"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="288724720"/>
+        <c:axId val="301016344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -670,7 +670,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="288723544"/>
+        <c:crossAx val="301017520"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -678,7 +678,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="288723544"/>
+        <c:axId val="301017520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -689,7 +689,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="288724720"/>
+        <c:crossAx val="301016344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -792,7 +792,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Habilis</c:v>
+                  <c:v>Gismo</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -843,11 +843,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="288727072"/>
-        <c:axId val="288723936"/>
+        <c:axId val="301017912"/>
+        <c:axId val="301011640"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="288727072"/>
+        <c:axId val="301017912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -857,7 +857,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="288723936"/>
+        <c:crossAx val="301011640"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -865,7 +865,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="288723936"/>
+        <c:axId val="301011640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -877,7 +877,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="288727072"/>
+        <c:crossAx val="301017912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -903,16 +903,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>42862</xdr:colOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>240982</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>52387</xdr:rowOff>
+      <xdr:rowOff>37147</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>347662</xdr:colOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>545782</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>185737</xdr:rowOff>
+      <xdr:rowOff>170497</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1295,55 +1295,55 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="C4" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="D4" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="E4" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="E4" s="5" t="s">
-        <v>29</v>
-      </c>
       <c r="I4" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="J4" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="J4" s="5" t="s">
+      <c r="K4" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="K4" s="5" t="s">
+      <c r="L4" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="L4" s="5" t="s">
+      <c r="M4" s="5" t="s">
         <v>28</v>
-      </c>
-      <c r="M4" s="5" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B5" s="3">
         <v>8</v>
@@ -1358,7 +1358,7 @@
         <v>4</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J5" s="3">
         <v>8</v>
@@ -1375,7 +1375,7 @@
     </row>
     <row r="6" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B6" s="4">
         <v>8</v>
@@ -1390,7 +1390,7 @@
         <v>5.3571428571428568</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J6" s="4">
         <v>8</v>
@@ -1407,59 +1407,59 @@
     </row>
     <row r="9" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="C10" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="D10" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="E10" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="E10" s="5" t="s">
+      <c r="F10" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="F10" s="5" t="s">
+      <c r="G10" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="G10" s="5" t="s">
-        <v>39</v>
-      </c>
       <c r="I10" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="J10" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="J10" s="5" t="s">
+      <c r="K10" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="K10" s="5" t="s">
+      <c r="L10" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="L10" s="5" t="s">
+      <c r="M10" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="M10" s="5" t="s">
+      <c r="N10" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="N10" s="5" t="s">
+      <c r="O10" s="5" t="s">
         <v>38</v>
-      </c>
-      <c r="O10" s="5" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B11" s="3">
         <v>2.25</v>
@@ -1480,7 +1480,7 @@
         <v>4.6001099366694227</v>
       </c>
       <c r="I11" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J11" s="3">
         <v>49</v>
@@ -1503,7 +1503,7 @@
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B12" s="3">
         <v>65.5</v>
@@ -1518,7 +1518,7 @@
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
       <c r="I12" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J12" s="3">
         <v>182.75</v>
@@ -1551,7 +1551,7 @@
     </row>
     <row r="14" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B14" s="4">
         <v>67.75</v>
@@ -1564,7 +1564,7 @@
       <c r="F14" s="4"/>
       <c r="G14" s="4"/>
       <c r="I14" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J14" s="4">
         <v>231.75</v>
@@ -1579,55 +1579,55 @@
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="19" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I19" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B20" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B20" s="5" t="s">
+      <c r="C20" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C20" s="5" t="s">
+      <c r="D20" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="D20" s="5" t="s">
+      <c r="E20" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="E20" s="5" t="s">
-        <v>29</v>
-      </c>
       <c r="I20" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="J20" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="J20" s="5" t="s">
+      <c r="K20" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="K20" s="5" t="s">
+      <c r="L20" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="L20" s="5" t="s">
+      <c r="M20" s="5" t="s">
         <v>28</v>
-      </c>
-      <c r="M20" s="5" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B21" s="3">
         <v>8</v>
@@ -1642,7 +1642,7 @@
         <v>12.571428571428571</v>
       </c>
       <c r="I21" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J21" s="3">
         <v>8</v>
@@ -1659,7 +1659,7 @@
     </row>
     <row r="22" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B22" s="4">
         <v>8</v>
@@ -1674,7 +1674,7 @@
         <v>13.642857142857142</v>
       </c>
       <c r="I22" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J22" s="4">
         <v>8</v>
@@ -1691,59 +1691,59 @@
     </row>
     <row r="25" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I25" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A26" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B26" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="B26" s="5" t="s">
+      <c r="C26" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="C26" s="5" t="s">
+      <c r="D26" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="D26" s="5" t="s">
+      <c r="E26" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="E26" s="5" t="s">
+      <c r="F26" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="F26" s="5" t="s">
+      <c r="G26" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="G26" s="5" t="s">
-        <v>39</v>
-      </c>
       <c r="I26" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="J26" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="J26" s="5" t="s">
+      <c r="K26" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="K26" s="5" t="s">
+      <c r="L26" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="L26" s="5" t="s">
+      <c r="M26" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="M26" s="5" t="s">
+      <c r="N26" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="N26" s="5" t="s">
+      <c r="O26" s="5" t="s">
         <v>38</v>
-      </c>
-      <c r="O26" s="5" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B27" s="3">
         <v>56.25</v>
@@ -1764,7 +1764,7 @@
         <v>4.6001099366694227</v>
       </c>
       <c r="I27" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J27" s="3">
         <v>4</v>
@@ -1787,7 +1787,7 @@
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B28" s="3">
         <v>183.5</v>
@@ -1802,7 +1802,7 @@
       <c r="F28" s="3"/>
       <c r="G28" s="3"/>
       <c r="I28" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J28" s="3">
         <v>67.75</v>
@@ -1835,7 +1835,7 @@
     </row>
     <row r="30" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B30" s="4">
         <v>239.75</v>
@@ -1848,7 +1848,7 @@
       <c r="F30" s="4"/>
       <c r="G30" s="4"/>
       <c r="I30" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J30" s="4">
         <v>71.75</v>
@@ -1882,22 +1882,22 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="5"/>
       <c r="B3" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3" s="5" t="s">
         <v>44</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B4" s="3">
         <v>14.5</v>
@@ -1908,7 +1908,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B5" s="3">
         <v>4</v>
@@ -1919,7 +1919,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B6" s="3">
         <v>8</v>
@@ -1930,7 +1930,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B7" s="3">
         <v>0</v>
@@ -1939,7 +1939,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B8" s="3">
         <v>14</v>
@@ -1948,7 +1948,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B9" s="3">
         <v>0.69348109601801777</v>
@@ -1957,7 +1957,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B10" s="3">
         <v>0.24967620533224472</v>
@@ -1966,7 +1966,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B11" s="3">
         <v>1.7613101357748921</v>
@@ -1975,7 +1975,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B12" s="3">
         <v>0.49935241066448943</v>
@@ -1984,7 +1984,7 @@
     </row>
     <row r="13" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B13" s="4">
         <v>2.1447866879178044</v>
@@ -2008,22 +2008,22 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="5"/>
       <c r="B3" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3" s="5" t="s">
         <v>44</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B4" s="3">
         <v>14.5</v>
@@ -2034,7 +2034,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B5" s="3">
         <v>4</v>
@@ -2045,7 +2045,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B6" s="3">
         <v>8</v>
@@ -2056,7 +2056,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B7" s="3">
         <v>9.2582009977255131E-2</v>
@@ -2065,7 +2065,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B8" s="3">
         <v>0</v>
@@ -2074,7 +2074,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B9" s="3">
         <v>7</v>
@@ -2083,7 +2083,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B10" s="3">
         <v>0.72760687510899891</v>
@@ -2092,7 +2092,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B11" s="3">
         <v>0.2452344580190246</v>
@@ -2101,7 +2101,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B12" s="3">
         <v>1.8945786050900073</v>
@@ -2110,7 +2110,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B13" s="3">
         <v>0.49046891603804921</v>
@@ -2119,7 +2119,7 @@
     </row>
     <row r="14" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B14" s="4">
         <v>2.3646242515927849</v>
@@ -2135,8 +2135,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C4" workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2680,12 +2680,12 @@
         <v>20</v>
       </c>
       <c r="L10" t="s">
-        <v>21</v>
+        <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>21</v>
+        <v>55</v>
       </c>
       <c r="B11">
         <f>AVERAGE(F2:F9)</f>
@@ -2704,7 +2704,7 @@
         <v>6.875</v>
       </c>
       <c r="J11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K11" s="1">
         <f>AVERAGE(K2:K9)</f>

</xml_diff>

<commit_message>
New figure, new text about design decisions
</commit_message>
<xml_diff>
--- a/HabilisX/890/HabilisData.xlsx
+++ b/HabilisX/890/HabilisData.xlsx
@@ -2135,8 +2135,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+    <sheetView tabSelected="1" topLeftCell="J21" workbookViewId="0">
+      <selection activeCell="V32" sqref="V32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>